<commit_message>
dtr login page add empdata amd factory
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempDtrLoginHistory.xlsx
+++ b/DKS-API/Resources/Template/TempDtrLoginHistory.xlsx
@@ -19,37 +19,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>System Name</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>LoginTime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.SystemName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.Account</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.LoginTime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.IP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.FactoryId</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Factory Id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Account</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LoginTime</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.SystemName</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.Account</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.LoginTime</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Work No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.WorkNo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.Name</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -58,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="yyyy/m/d\ h:mm;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d\ h:mm;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -128,13 +152,13 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -463,47 +487,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" style="5" customWidth="1"/>
-    <col min="4" max="4" width="84.85546875" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="5" width="12.5703125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="21" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="D2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>